<commit_message>
add flags; edit sql schem
</commit_message>
<xml_diff>
--- a/database/data_quizzes.xlsx
+++ b/database/data_quizzes.xlsx
@@ -8,19 +8,32 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maela\Documents\Projets\Dev\Web\Courses\terraquiz\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7BD7A41-62C7-417F-8D89-7185F7850541}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7C40CDE-1EDC-4EC6-B4CC-855A1E64FF19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-78" yWindow="0" windowWidth="12054" windowHeight="12318" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1086" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1628" uniqueCount="486">
   <si>
     <t>flag</t>
   </si>
@@ -698,6 +711,786 @@
   </si>
   <si>
     <t>republic_of_the_congo</t>
+  </si>
+  <si>
+    <t>af</t>
+  </si>
+  <si>
+    <t>Afrikaans</t>
+  </si>
+  <si>
+    <t>Ek is lief vir die reuk van vars brood.</t>
+  </si>
+  <si>
+    <t>English</t>
+  </si>
+  <si>
+    <t>French</t>
+  </si>
+  <si>
+    <t>German</t>
+  </si>
+  <si>
+    <t>ar</t>
+  </si>
+  <si>
+    <t>Arabic</t>
+  </si>
+  <si>
+    <t>العلم يعطي الحكمة.</t>
+  </si>
+  <si>
+    <t>Spanish</t>
+  </si>
+  <si>
+    <t>az</t>
+  </si>
+  <si>
+    <t>Azeri</t>
+  </si>
+  <si>
+    <t>Səmimi gülmə insanın ürəyini açar.</t>
+  </si>
+  <si>
+    <t>Turkish</t>
+  </si>
+  <si>
+    <t>Russian</t>
+  </si>
+  <si>
+    <t>be</t>
+  </si>
+  <si>
+    <t>Belarusian</t>
+  </si>
+  <si>
+    <t>Мудрасць - у самасаведамасці.</t>
+  </si>
+  <si>
+    <t>Ukrainian</t>
+  </si>
+  <si>
+    <t>Polish</t>
+  </si>
+  <si>
+    <t>ca</t>
+  </si>
+  <si>
+    <t>Catalan</t>
+  </si>
+  <si>
+    <t>El gat està dormint a la butxaca.</t>
+  </si>
+  <si>
+    <t>Italian</t>
+  </si>
+  <si>
+    <t>cs</t>
+  </si>
+  <si>
+    <t>Czech</t>
+  </si>
+  <si>
+    <t>Čas je nejlepší lék.</t>
+  </si>
+  <si>
+    <t>Slovak</t>
+  </si>
+  <si>
+    <t>da</t>
+  </si>
+  <si>
+    <t>Danish</t>
+  </si>
+  <si>
+    <t>Solen skinner på den blå himmel.</t>
+  </si>
+  <si>
+    <t>Swedish</t>
+  </si>
+  <si>
+    <t>Norwegian</t>
+  </si>
+  <si>
+    <t>de</t>
+  </si>
+  <si>
+    <t>Die Welt ist ein Buch. Wer nie reist, sieht nur eine Seite davon.</t>
+  </si>
+  <si>
+    <t>el</t>
+  </si>
+  <si>
+    <t>Greek</t>
+  </si>
+  <si>
+    <t>Η γνώση είναι φως και η άγνοια είναι σκοτάδι.</t>
+  </si>
+  <si>
+    <t>en</t>
+  </si>
+  <si>
+    <t>Time flies when you're having fun.</t>
+  </si>
+  <si>
+    <t>es</t>
+  </si>
+  <si>
+    <t>La vida es un sueño, y los sueños, sueños son.</t>
+  </si>
+  <si>
+    <t>et</t>
+  </si>
+  <si>
+    <t>Estonian</t>
+  </si>
+  <si>
+    <t>Õnn naeratab neile, kes ootavad.</t>
+  </si>
+  <si>
+    <t>Finnish</t>
+  </si>
+  <si>
+    <t>Latvian</t>
+  </si>
+  <si>
+    <t>Lithuanian</t>
+  </si>
+  <si>
+    <t>eu</t>
+  </si>
+  <si>
+    <t>Basque</t>
+  </si>
+  <si>
+    <t>Txoria txori da.</t>
+  </si>
+  <si>
+    <t>fa</t>
+  </si>
+  <si>
+    <t>Farsi</t>
+  </si>
+  <si>
+    <t>آرامش در دل انسان به روزهای بی کاری می‌آید.</t>
+  </si>
+  <si>
+    <t>Urdu</t>
+  </si>
+  <si>
+    <t>fi</t>
+  </si>
+  <si>
+    <t>Elämä on kuin polkupyörä. Jotta pysyisi tasapainossa, on liikuttava eteenpäin.</t>
+  </si>
+  <si>
+    <t>fr</t>
+  </si>
+  <si>
+    <t>La vie est belle.</t>
+  </si>
+  <si>
+    <t>gl</t>
+  </si>
+  <si>
+    <t>Galician</t>
+  </si>
+  <si>
+    <t>A lingua é a patria.</t>
+  </si>
+  <si>
+    <t>Portuguese</t>
+  </si>
+  <si>
+    <t>gu</t>
+  </si>
+  <si>
+    <t>Gujarati</t>
+  </si>
+  <si>
+    <t>વિદ્યા વિના જીવન અદૂર છે.</t>
+  </si>
+  <si>
+    <t>Hindi</t>
+  </si>
+  <si>
+    <t>Marathi</t>
+  </si>
+  <si>
+    <t>Punjabi</t>
+  </si>
+  <si>
+    <t>he</t>
+  </si>
+  <si>
+    <t>Hebrew</t>
+  </si>
+  <si>
+    <t>הבשורה על פי מתי.</t>
+  </si>
+  <si>
+    <t>Yiddish</t>
+  </si>
+  <si>
+    <t>hi</t>
+  </si>
+  <si>
+    <t>सपने वो नहीं जो हम सोते समय देखते हैं, सपने वो हैं जो हमें सोने नहीं देते</t>
+  </si>
+  <si>
+    <t>Bengali</t>
+  </si>
+  <si>
+    <t>hr</t>
+  </si>
+  <si>
+    <t>Croatian</t>
+  </si>
+  <si>
+    <t>Znanje je ključ uspjeha.</t>
+  </si>
+  <si>
+    <t>Slovenian</t>
+  </si>
+  <si>
+    <t>Serbian</t>
+  </si>
+  <si>
+    <t>Bosnian</t>
+  </si>
+  <si>
+    <t>hu</t>
+  </si>
+  <si>
+    <t>Hungarian</t>
+  </si>
+  <si>
+    <t>Az élet szép, mint a virágok.</t>
+  </si>
+  <si>
+    <t>Romanian</t>
+  </si>
+  <si>
+    <t>hy</t>
+  </si>
+  <si>
+    <t>Armenian</t>
+  </si>
+  <si>
+    <t>Գիտելիքը զինվորվում է ամեն դեպի բարձրություն.</t>
+  </si>
+  <si>
+    <t>Georgian</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>Indonesian</t>
+  </si>
+  <si>
+    <t>Hidup adalah seni, dan setiap orang seniman.</t>
+  </si>
+  <si>
+    <t>Malay</t>
+  </si>
+  <si>
+    <t>Filipino</t>
+  </si>
+  <si>
+    <t>Javanese</t>
+  </si>
+  <si>
+    <t>is</t>
+  </si>
+  <si>
+    <t>Icelandic</t>
+  </si>
+  <si>
+    <t>Það er enginn hollusta nema heilsa.</t>
+  </si>
+  <si>
+    <t>it</t>
+  </si>
+  <si>
+    <t>La vita è un sogno, e sognare è vivere due volte.</t>
+  </si>
+  <si>
+    <t>ja</t>
+  </si>
+  <si>
+    <t>Japanese</t>
+  </si>
+  <si>
+    <t>虎穴に入らずんば虎子を得ず。</t>
+  </si>
+  <si>
+    <t>Chinese</t>
+  </si>
+  <si>
+    <t>Korean</t>
+  </si>
+  <si>
+    <t>Vietnamese</t>
+  </si>
+  <si>
+    <t>ka</t>
+  </si>
+  <si>
+    <t>გონება სულს დაეხმარება.</t>
+  </si>
+  <si>
+    <t>Azerbaijani</t>
+  </si>
+  <si>
+    <t>kk</t>
+  </si>
+  <si>
+    <t>Kazakh</t>
+  </si>
+  <si>
+    <t>Білім мәнен жүр.</t>
+  </si>
+  <si>
+    <t>Kyrgyz</t>
+  </si>
+  <si>
+    <t>Uzbek</t>
+  </si>
+  <si>
+    <t>Tatar</t>
+  </si>
+  <si>
+    <t>kn</t>
+  </si>
+  <si>
+    <t>Kannada</t>
+  </si>
+  <si>
+    <t>ಹಸಿವಿನಿಂದ ಹುಟ್ಟುವ ಹುಳು ಮೇಲಿದೆ.</t>
+  </si>
+  <si>
+    <t>Telugu</t>
+  </si>
+  <si>
+    <t>Tamil</t>
+  </si>
+  <si>
+    <t>Malayalam</t>
+  </si>
+  <si>
+    <t>ko</t>
+  </si>
+  <si>
+    <t>지식은 힘입니다.</t>
+  </si>
+  <si>
+    <t>kok</t>
+  </si>
+  <si>
+    <t>Konkani</t>
+  </si>
+  <si>
+    <t>मनस्सांतां फल वाहून घ्यावं.</t>
+  </si>
+  <si>
+    <t>ky</t>
+  </si>
+  <si>
+    <t>Билим бир алдымдың казынасы болсо да, ондай болгонун күмөнү болуш абзалдык.</t>
+  </si>
+  <si>
+    <t>Tajik</t>
+  </si>
+  <si>
+    <t>lt</t>
+  </si>
+  <si>
+    <t>Išmintis - tai geriausias turtas.</t>
+  </si>
+  <si>
+    <t>lv</t>
+  </si>
+  <si>
+    <t>Zināšanas ir spēks.</t>
+  </si>
+  <si>
+    <t>mi</t>
+  </si>
+  <si>
+    <t>Maori</t>
+  </si>
+  <si>
+    <t>He aha te mea nui o te ao? He tangata, he tangata, he tangata.</t>
+  </si>
+  <si>
+    <t>Samoan</t>
+  </si>
+  <si>
+    <t>Tongan</t>
+  </si>
+  <si>
+    <t>mk</t>
+  </si>
+  <si>
+    <t>FYRO Macedonian</t>
+  </si>
+  <si>
+    <t>Знаењето е силата.</t>
+  </si>
+  <si>
+    <t>Bulgarian</t>
+  </si>
+  <si>
+    <t>mn</t>
+  </si>
+  <si>
+    <t>Mongolian</t>
+  </si>
+  <si>
+    <t>Мэргэжил нь оршин суугаа бол хамгийн сайн ижил байгууллага.</t>
+  </si>
+  <si>
+    <t>mr</t>
+  </si>
+  <si>
+    <t>ज्ञानाने संग्रह केलेलं काम कधीचित्कार न करता.</t>
+  </si>
+  <si>
+    <t>ms</t>
+  </si>
+  <si>
+    <t>Ilmu adalah harta yang paling berharga.</t>
+  </si>
+  <si>
+    <t>mt</t>
+  </si>
+  <si>
+    <t>Maltese</t>
+  </si>
+  <si>
+    <t>L-isforz ta' l-edukazzjoni huwa l-arma l-aktar qawwija li tista' ssib.</t>
+  </si>
+  <si>
+    <t>nb</t>
+  </si>
+  <si>
+    <t>Kunnskap er makt.</t>
+  </si>
+  <si>
+    <t>nl</t>
+  </si>
+  <si>
+    <t>Dutch</t>
+  </si>
+  <si>
+    <t>Kennis is macht.</t>
+  </si>
+  <si>
+    <t>nn-NO</t>
+  </si>
+  <si>
+    <t>Kunnskap er nøkkelen til suksess.</t>
+  </si>
+  <si>
+    <t>ns</t>
+  </si>
+  <si>
+    <t>Northern Sotho</t>
+  </si>
+  <si>
+    <t>Tshedza ke go tlhokomela bogosi.</t>
+  </si>
+  <si>
+    <t>Zulu</t>
+  </si>
+  <si>
+    <t>Xhosa</t>
+  </si>
+  <si>
+    <t>Tswana</t>
+  </si>
+  <si>
+    <t>pa</t>
+  </si>
+  <si>
+    <t>ਜਾਣਕਾਰੀ ਸਬ ਤੋਂ ਵੱਡਾ ਸਮ੍ਹਾਲਾ ਹੈ.</t>
+  </si>
+  <si>
+    <t>pl</t>
+  </si>
+  <si>
+    <t>Wiedza to potęga.</t>
+  </si>
+  <si>
+    <t>ps</t>
+  </si>
+  <si>
+    <t>Pashto</t>
+  </si>
+  <si>
+    <t>ځان او پوه ځان ژوند دې په ارمانو کې دې.</t>
+  </si>
+  <si>
+    <t>Persian</t>
+  </si>
+  <si>
+    <t>pt</t>
+  </si>
+  <si>
+    <t>A sabedoria é a principal riqueza.</t>
+  </si>
+  <si>
+    <t>qu</t>
+  </si>
+  <si>
+    <t>Quechua</t>
+  </si>
+  <si>
+    <t>Yuyaypaqmi ñuqaqa yanapaq.</t>
+  </si>
+  <si>
+    <t>ro</t>
+  </si>
+  <si>
+    <t>Cunoașterea este putere.</t>
+  </si>
+  <si>
+    <t>ru</t>
+  </si>
+  <si>
+    <t>Знание - сила.</t>
+  </si>
+  <si>
+    <t>sa</t>
+  </si>
+  <si>
+    <t>Sanskrit</t>
+  </si>
+  <si>
+    <t>विद्या ददाति विनयं.</t>
+  </si>
+  <si>
+    <t>se</t>
+  </si>
+  <si>
+    <t>Sami</t>
+  </si>
+  <si>
+    <t>Dáidda lea fámu.</t>
+  </si>
+  <si>
+    <t>sk</t>
+  </si>
+  <si>
+    <t>Vedomosti sú sila.</t>
+  </si>
+  <si>
+    <t>sl</t>
+  </si>
+  <si>
+    <t>Znanje je moč.</t>
+  </si>
+  <si>
+    <t>sq</t>
+  </si>
+  <si>
+    <t>Albanian</t>
+  </si>
+  <si>
+    <t>Dija është fuqi.</t>
+  </si>
+  <si>
+    <t>sr-BA</t>
+  </si>
+  <si>
+    <t>Знање је светло у тами.</t>
+  </si>
+  <si>
+    <t>Montenegrin</t>
+  </si>
+  <si>
+    <t>sv</t>
+  </si>
+  <si>
+    <t>Kunskap är makt.</t>
+  </si>
+  <si>
+    <t>sw</t>
+  </si>
+  <si>
+    <t>Swahili</t>
+  </si>
+  <si>
+    <t>Maarifa ni nguvu.</t>
+  </si>
+  <si>
+    <t>syr</t>
+  </si>
+  <si>
+    <t>Syriac</t>
+  </si>
+  <si>
+    <t>ܫܠܡܐ ܬܪܥܐ ܘܬܒܘܚܐ ܐܦ ܡܕܡܢܚܐ ܩܕܝܡܐ.</t>
+  </si>
+  <si>
+    <t>Assyrian</t>
+  </si>
+  <si>
+    <t>ta</t>
+  </si>
+  <si>
+    <t>அறிவு ஆற்றுவது மிகுந்த ஐசுவார்த்தியம்.</t>
+  </si>
+  <si>
+    <t>te</t>
+  </si>
+  <si>
+    <t>పరిజ్ఞానం శక్తి.</t>
+  </si>
+  <si>
+    <t>th</t>
+  </si>
+  <si>
+    <t>Thai</t>
+  </si>
+  <si>
+    <t>ความรู้คือพลัง.</t>
+  </si>
+  <si>
+    <t>tl</t>
+  </si>
+  <si>
+    <t>Tagalog</t>
+  </si>
+  <si>
+    <t>Ang edukasyon ay susi sa tagumpay.</t>
+  </si>
+  <si>
+    <t>tn</t>
+  </si>
+  <si>
+    <t>Tshwaragano ke kgomo ya bolwetsi.</t>
+  </si>
+  <si>
+    <t>Sotho</t>
+  </si>
+  <si>
+    <t>tr</t>
+  </si>
+  <si>
+    <t>Bilgi güçtür.</t>
+  </si>
+  <si>
+    <t>tt</t>
+  </si>
+  <si>
+    <t>Белем - аңыз.</t>
+  </si>
+  <si>
+    <t>ts</t>
+  </si>
+  <si>
+    <t>Tsonga</t>
+  </si>
+  <si>
+    <t>Ku dyondzisa ku nghena emhlabeni.</t>
+  </si>
+  <si>
+    <t>Swazi</t>
+  </si>
+  <si>
+    <t>uk</t>
+  </si>
+  <si>
+    <t>Знання - це сила.</t>
+  </si>
+  <si>
+    <t>ur</t>
+  </si>
+  <si>
+    <t>علم سے زندگی میں اتنی کامیابی آتی ہے جیسے روشنی کے ساتھ رات میں نکلنا۔</t>
+  </si>
+  <si>
+    <t>uz</t>
+  </si>
+  <si>
+    <t>Bilim kuchdir.</t>
+  </si>
+  <si>
+    <t>Turkmen</t>
+  </si>
+  <si>
+    <t>vi</t>
+  </si>
+  <si>
+    <t>Tri thức là sức mạnh.</t>
+  </si>
+  <si>
+    <t>xh</t>
+  </si>
+  <si>
+    <t>Ukufunda kuyiindlela yokwenza imisebenzi emihle.</t>
+  </si>
+  <si>
+    <t>zh</t>
+  </si>
+  <si>
+    <t>知识改变命运。</t>
+  </si>
+  <si>
+    <t>zu</t>
+  </si>
+  <si>
+    <t>Ukufunda akukhomba amathuba.</t>
+  </si>
+  <si>
+    <t>Hausa</t>
+  </si>
+  <si>
+    <t>Igbo</t>
+  </si>
+  <si>
+    <t>Wolof</t>
+  </si>
+  <si>
+    <t>Yoruba</t>
+  </si>
+  <si>
+    <t>Sinhala</t>
+  </si>
+  <si>
+    <t>Irish</t>
+  </si>
+  <si>
+    <t>Macedonian</t>
+  </si>
+  <si>
+    <t>Fijian</t>
+  </si>
+  <si>
+    <t>Hawaiian</t>
+  </si>
+  <si>
+    <t>continent</t>
+  </si>
+  <si>
+    <t>Africa</t>
+  </si>
+  <si>
+    <t>Asia</t>
+  </si>
+  <si>
+    <t>Europe</t>
+  </si>
+  <si>
+    <t>North America</t>
+  </si>
+  <si>
+    <t>South America</t>
+  </si>
+  <si>
+    <t>Oceania</t>
   </si>
 </sst>
 </file>
@@ -1580,10 +2373,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AI51"/>
+  <dimension ref="A1:AS133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H49" sqref="H49"/>
+    <sheetView tabSelected="1" topLeftCell="A104" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N125" sqref="N125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1602,7 +2395,9 @@
     <col min="32" max="32" width="11.20703125" style="2" customWidth="1"/>
     <col min="33" max="33" width="12.20703125" style="2" customWidth="1"/>
     <col min="34" max="34" width="11.68359375" style="2" customWidth="1"/>
-    <col min="35" max="16384" width="8.83984375" style="2"/>
+    <col min="35" max="43" width="8.83984375" style="2"/>
+    <col min="44" max="44" width="9" style="2" customWidth="1"/>
+    <col min="46" max="16384" width="8.83984375" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:35" x14ac:dyDescent="0.55000000000000004">
@@ -5776,23 +6571,1817 @@
       <c r="H51" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="I51" s="2" t="s">
+        <v>479</v>
+      </c>
+      <c r="L51" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="M51" s="2" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="52" spans="2:28" x14ac:dyDescent="0.55000000000000004">
+      <c r="B52" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="F52" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="G52" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="I52" s="2" t="str">
+        <f>VLOOKUP(C52, $L$51:$M$69,  2)</f>
+        <v>Africa</v>
+      </c>
+      <c r="L52" s="2" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="53" spans="2:28" x14ac:dyDescent="0.55000000000000004">
+      <c r="B53" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="E53" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="F53" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="G53" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="L53" s="2" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="54" spans="2:28" x14ac:dyDescent="0.55000000000000004">
+      <c r="B54" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="E54" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="F54" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="G54" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="L54" s="2" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="55" spans="2:28" x14ac:dyDescent="0.55000000000000004">
+      <c r="B55" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="E55" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="F55" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="G55" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="L55" s="2" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="56" spans="2:28" x14ac:dyDescent="0.55000000000000004">
+      <c r="B56" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="E56" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="F56" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="G56" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="L56" s="2" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="57" spans="2:28" x14ac:dyDescent="0.55000000000000004">
+      <c r="B57" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="E57" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="F57" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="G57" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="L57" s="2" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="58" spans="2:28" x14ac:dyDescent="0.55000000000000004">
+      <c r="B58" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="E58" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="F58" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="G58" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="L58" s="2" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="59" spans="2:28" x14ac:dyDescent="0.55000000000000004">
+      <c r="B59" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="E59" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="F59" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="G59" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="L59" s="2" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="60" spans="2:28" x14ac:dyDescent="0.55000000000000004">
+      <c r="B60" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="E60" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="F60" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="G60" s="2" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="61" spans="2:28" x14ac:dyDescent="0.55000000000000004">
+      <c r="B61" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="E61" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="F61" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="G61" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="L61" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="M61" s="2" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="62" spans="2:28" x14ac:dyDescent="0.55000000000000004">
+      <c r="B62" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="E62" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="F62" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="G62" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="L62" s="2" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="63" spans="2:28" x14ac:dyDescent="0.55000000000000004">
+      <c r="B63" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="E63" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="F63" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="G63" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="L63" s="2" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="64" spans="2:28" x14ac:dyDescent="0.55000000000000004">
+      <c r="B64" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="D64" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="E64" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="F64" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="G64" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="L64" s="2" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="65" spans="2:40" x14ac:dyDescent="0.55000000000000004">
+      <c r="B65" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="D65" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="E65" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="F65" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="G65" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="L65" s="2" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="66" spans="2:40" x14ac:dyDescent="0.55000000000000004">
+      <c r="B66" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="D66" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="E66" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="F66" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="G66" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="L66" s="2" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="67" spans="2:40" x14ac:dyDescent="0.55000000000000004">
+      <c r="B67" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="D67" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="E67" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="F67" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="G67" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="L67" s="2" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="68" spans="2:40" x14ac:dyDescent="0.55000000000000004">
+      <c r="B68" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="D68" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="E68" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="F68" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="G68" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="L68" s="2" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="69" spans="2:40" x14ac:dyDescent="0.55000000000000004">
+      <c r="B69" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="D69" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="E69" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="F69" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="G69" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="L69" s="2" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="70" spans="2:40" x14ac:dyDescent="0.55000000000000004">
+      <c r="B70" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="D70" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="E70" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="F70" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="G70" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="L70" s="2" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="71" spans="2:40" x14ac:dyDescent="0.55000000000000004">
+      <c r="B71" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="D71" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="E71" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="F71" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="G71" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="L71" s="2" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="72" spans="2:40" x14ac:dyDescent="0.55000000000000004">
+      <c r="B72" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="D72" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="E72" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="F72" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="G72" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="L72" s="2" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="73" spans="2:40" x14ac:dyDescent="0.55000000000000004">
+      <c r="B73" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="D73" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="E73" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="F73" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="G73" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="L73" s="2" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="74" spans="2:40" x14ac:dyDescent="0.55000000000000004">
+      <c r="B74" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="E74" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="F74" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="G74" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="L74" s="2" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="75" spans="2:40" x14ac:dyDescent="0.55000000000000004">
+      <c r="B75" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="E75" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="F75" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="G75" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="L75" s="2" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="76" spans="2:40" x14ac:dyDescent="0.55000000000000004">
+      <c r="B76" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="D76" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="E76" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="F76" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="G76" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="L76" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="AN76" s="2" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="77" spans="2:40" x14ac:dyDescent="0.55000000000000004">
+      <c r="B77" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="C77" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="D77" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="E77" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="F77" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="G77" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="L77" s="2" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="78" spans="2:40" x14ac:dyDescent="0.55000000000000004">
+      <c r="B78" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="C78" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="D78" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="E78" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="F78" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="G78" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="L78" s="2" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="79" spans="2:40" x14ac:dyDescent="0.55000000000000004">
+      <c r="B79" s="2" t="s">
+        <v>334</v>
+      </c>
+      <c r="C79" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="D79" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="E79" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="F79" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="G79" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="L79" s="2" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="80" spans="2:40" x14ac:dyDescent="0.55000000000000004">
+      <c r="B80" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="D80" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="E80" s="2" t="s">
+        <v>339</v>
+      </c>
+      <c r="F80" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="G80" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="L80" s="2" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="81" spans="2:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="B81" s="2" t="s">
+        <v>344</v>
+      </c>
+      <c r="C81" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="D81" s="2" t="s">
+        <v>342</v>
+      </c>
+      <c r="E81" s="2" t="s">
+        <v>345</v>
+      </c>
+      <c r="F81" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="G81" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="L81" s="2" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="82" spans="2:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="B82" s="2" t="s">
+        <v>349</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="D82" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="E82" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="F82" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="G82" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="L82" s="2" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="83" spans="2:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="B83" s="2" t="s">
+        <v>352</v>
+      </c>
+      <c r="C83" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="D83" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="E83" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="F83" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="G83" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="84" spans="2:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="B84" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="C84" s="2" t="s">
+        <v>339</v>
+      </c>
+      <c r="D84" s="2" t="s">
+        <v>353</v>
+      </c>
+      <c r="E84" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="F84" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="G84" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="L84" s="2" t="s">
+        <v>420</v>
+      </c>
+      <c r="M84" s="2" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="85" spans="2:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="B85" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="C85" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="D85" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="E85" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="F85" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="G85" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="L85" s="2" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="86" spans="2:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="B86" s="2" t="s">
+        <v>359</v>
+      </c>
+      <c r="C86" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="D86" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="E86" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="F86" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="G86" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="L86" s="2" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="87" spans="2:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="B87" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="C87" s="2" t="s">
+        <v>361</v>
+      </c>
+      <c r="D87" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="E87" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="F87" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="G87" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="L87" s="2" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="88" spans="2:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="B88" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="C88" s="2" t="s">
+        <v>366</v>
+      </c>
+      <c r="D88" s="2" t="s">
+        <v>365</v>
+      </c>
+      <c r="E88" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="F88" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="G88" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="L88" s="2" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="89" spans="2:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="B89" s="2" t="s">
+        <v>371</v>
+      </c>
+      <c r="C89" s="2" t="s">
+        <v>370</v>
+      </c>
+      <c r="D89" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="E89" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="F89" s="2" t="s">
+        <v>339</v>
+      </c>
+      <c r="G89" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="L89" s="2" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="90" spans="2:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="B90" s="2" t="s">
+        <v>373</v>
+      </c>
+      <c r="C90" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="D90" s="2" t="s">
+        <v>372</v>
+      </c>
+      <c r="E90" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="F90" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="G90" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="L90" s="2" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="91" spans="2:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="B91" s="2" t="s">
+        <v>375</v>
+      </c>
+      <c r="C91" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="D91" s="2" t="s">
+        <v>374</v>
+      </c>
+      <c r="E91" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="F91" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="G91" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="L91" s="2" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="92" spans="2:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="B92" s="2" t="s">
+        <v>378</v>
+      </c>
+      <c r="C92" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="D92" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="E92" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="F92" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="G92" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="L92" s="2" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="93" spans="2:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="B93" s="2" t="s">
+        <v>380</v>
+      </c>
+      <c r="C93" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="D93" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="E93" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="F93" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="G93" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="L93" s="2" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="94" spans="2:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="B94" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="C94" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="D94" s="2" t="s">
+        <v>381</v>
+      </c>
+      <c r="E94" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="F94" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="G94" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="L94" s="2" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="95" spans="2:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="B95" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="C95" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="D95" s="2" t="s">
+        <v>384</v>
+      </c>
+      <c r="E95" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="F95" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="G95" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="L95" s="2" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="96" spans="2:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="B96" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="C96" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="D96" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="E96" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="F96" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="G96" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="L96" s="2" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="97" spans="2:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="B97" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="C97" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="D97" s="2" t="s">
+        <v>392</v>
+      </c>
+      <c r="E97" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="F97" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="G97" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="L97" s="2" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="98" spans="2:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="B98" s="2" t="s">
+        <v>395</v>
+      </c>
+      <c r="C98" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="D98" s="2" t="s">
+        <v>394</v>
+      </c>
+      <c r="E98" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="F98" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="G98" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="L98" s="2" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="99" spans="2:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="B99" s="2" t="s">
+        <v>398</v>
+      </c>
+      <c r="C99" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="D99" s="2" t="s">
+        <v>396</v>
+      </c>
+      <c r="E99" s="2" t="s">
+        <v>399</v>
+      </c>
+      <c r="F99" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="G99" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="L99" s="2" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="100" spans="2:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="B100" s="2" t="s">
+        <v>401</v>
+      </c>
+      <c r="C100" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="D100" s="2" t="s">
+        <v>400</v>
+      </c>
+      <c r="E100" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="F100" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="G100" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="L100" s="2" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="101" spans="2:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="B101" s="2" t="s">
+        <v>404</v>
+      </c>
+      <c r="C101" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="D101" s="2" t="s">
+        <v>402</v>
+      </c>
+      <c r="E101" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="F101" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="G101" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="L101" s="2" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="102" spans="2:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="B102" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="C102" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="D102" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="E102" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="F102" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="G102" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="L102" s="2" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="103" spans="2:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="B103" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="C103" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="D103" s="2" t="s">
+        <v>407</v>
+      </c>
+      <c r="E103" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="F103" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="G103" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="L103" s="2" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="104" spans="2:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="B104" s="2" t="s">
+        <v>411</v>
+      </c>
+      <c r="C104" s="2" t="s">
+        <v>410</v>
+      </c>
+      <c r="D104" s="2" t="s">
+        <v>409</v>
+      </c>
+      <c r="E104" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="F104" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="G104" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="L104" s="2" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="105" spans="2:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="B105" s="2" t="s">
+        <v>414</v>
+      </c>
+      <c r="C105" s="2" t="s">
+        <v>413</v>
+      </c>
+      <c r="D105" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="E105" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="F105" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="G105" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="L105" s="2" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="106" spans="2:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="B106" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="C106" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="D106" s="2" t="s">
+        <v>415</v>
+      </c>
+      <c r="E106" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="F106" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="G106" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="L106" s="2" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="107" spans="2:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="B107" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="C107" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="D107" s="2" t="s">
+        <v>417</v>
+      </c>
+      <c r="E107" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="F107" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="G107" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="L107" s="2" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="108" spans="2:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="B108" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="C108" s="2" t="s">
+        <v>420</v>
+      </c>
+      <c r="D108" s="2" t="s">
+        <v>419</v>
+      </c>
+      <c r="E108" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="F108" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="G108" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="L108" s="2" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="109" spans="2:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="B109" s="2" t="s">
+        <v>423</v>
+      </c>
+      <c r="C109" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="D109" s="2" t="s">
+        <v>422</v>
+      </c>
+      <c r="E109" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="F109" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="G109" s="2" t="s">
+        <v>424</v>
+      </c>
+      <c r="L109" s="2" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="110" spans="2:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="B110" s="2" t="s">
+        <v>426</v>
+      </c>
+      <c r="C110" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="D110" s="2" t="s">
+        <v>425</v>
+      </c>
+      <c r="E110" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="F110" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="G110" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="L110" s="2" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="111" spans="2:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="B111" s="2" t="s">
+        <v>429</v>
+      </c>
+      <c r="C111" s="2" t="s">
+        <v>428</v>
+      </c>
+      <c r="D111" s="2" t="s">
+        <v>427</v>
+      </c>
+      <c r="E111" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="F111" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="G111" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="L111" s="2" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="112" spans="2:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="B112" s="2" t="s">
+        <v>432</v>
+      </c>
+      <c r="C112" s="2" t="s">
+        <v>431</v>
+      </c>
+      <c r="D112" s="2" t="s">
+        <v>430</v>
+      </c>
+      <c r="E112" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="F112" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="G112" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="L112" s="2" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="113" spans="2:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="B113" s="2" t="s">
+        <v>435</v>
+      </c>
+      <c r="C113" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="D113" s="2" t="s">
+        <v>434</v>
+      </c>
+      <c r="E113" s="2" t="s">
+        <v>345</v>
+      </c>
+      <c r="F113" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="G113" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="L113" s="2" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="114" spans="2:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="B114" s="2" t="s">
+        <v>437</v>
+      </c>
+      <c r="C114" s="2" t="s">
+        <v>345</v>
+      </c>
+      <c r="D114" s="2" t="s">
+        <v>436</v>
+      </c>
+      <c r="E114" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="F114" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="G114" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="L114" s="2" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="115" spans="2:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="B115" s="2" t="s">
+        <v>440</v>
+      </c>
+      <c r="C115" s="2" t="s">
+        <v>439</v>
+      </c>
+      <c r="D115" s="2" t="s">
+        <v>438</v>
+      </c>
+      <c r="E115" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="F115" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="G115" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="L115" s="2" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="116" spans="2:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="B116" s="2" t="s">
+        <v>443</v>
+      </c>
+      <c r="C116" s="2" t="s">
+        <v>442</v>
+      </c>
+      <c r="D116" s="2" t="s">
+        <v>441</v>
+      </c>
+      <c r="E116" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="F116" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="G116" s="2" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="117" spans="2:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="B117" s="2" t="s">
+        <v>445</v>
+      </c>
+      <c r="C117" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="D117" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="E117" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="F117" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="G117" s="2" t="s">
+        <v>446</v>
+      </c>
+      <c r="L117" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="M117" s="2" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="118" spans="2:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="B118" s="2" t="s">
+        <v>448</v>
+      </c>
+      <c r="C118" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="D118" s="2" t="s">
+        <v>447</v>
+      </c>
+      <c r="E118" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="F118" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="G118" s="2" t="s">
+        <v>339</v>
+      </c>
+      <c r="L118" s="2" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="119" spans="2:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="B119" s="2" t="s">
+        <v>450</v>
+      </c>
+      <c r="C119" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="D119" s="2" t="s">
+        <v>449</v>
+      </c>
+      <c r="E119" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="F119" s="2" t="s">
+        <v>339</v>
+      </c>
+      <c r="G119" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="L119" s="2" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="120" spans="2:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="B120" s="2" t="s">
+        <v>453</v>
+      </c>
+      <c r="C120" s="2" t="s">
+        <v>452</v>
+      </c>
+      <c r="D120" s="2" t="s">
+        <v>451</v>
+      </c>
+      <c r="E120" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="F120" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="G120" s="2" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="121" spans="2:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="B121" s="2" t="s">
+        <v>456</v>
+      </c>
+      <c r="C121" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="D121" s="2" t="s">
+        <v>455</v>
+      </c>
+      <c r="E121" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="F121" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="G121" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="L121" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="M121" s="2" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="122" spans="2:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="B122" s="2" t="s">
+        <v>458</v>
+      </c>
+      <c r="C122" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="D122" s="2" t="s">
+        <v>457</v>
+      </c>
+      <c r="E122" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="F122" s="2" t="s">
+        <v>399</v>
+      </c>
+      <c r="G122" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="L122" s="2" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="123" spans="2:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="B123" s="2" t="s">
+        <v>460</v>
+      </c>
+      <c r="C123" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="D123" s="2" t="s">
+        <v>459</v>
+      </c>
+      <c r="E123" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="F123" s="2" t="s">
+        <v>339</v>
+      </c>
+      <c r="G123" s="2" t="s">
+        <v>461</v>
+      </c>
+      <c r="L123" s="2" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="124" spans="2:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="B124" s="2" t="s">
+        <v>463</v>
+      </c>
+      <c r="C124" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="D124" s="2" t="s">
+        <v>462</v>
+      </c>
+      <c r="E124" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="F124" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="G124" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="L124" s="2" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="125" spans="2:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="B125" s="2" t="s">
+        <v>465</v>
+      </c>
+      <c r="C125" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="D125" s="2" t="s">
+        <v>464</v>
+      </c>
+      <c r="E125" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="F125" s="2" t="s">
+        <v>446</v>
+      </c>
+      <c r="G125" s="2" t="s">
+        <v>454</v>
+      </c>
+      <c r="L125" s="2" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="126" spans="2:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="B126" s="2" t="s">
+        <v>467</v>
+      </c>
+      <c r="C126" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="D126" s="2" t="s">
+        <v>466</v>
+      </c>
+      <c r="E126" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="F126" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="G126" s="2" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="127" spans="2:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="B127" s="2" t="s">
+        <v>469</v>
+      </c>
+      <c r="C127" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="D127" s="2" t="s">
+        <v>468</v>
+      </c>
+      <c r="E127" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="F127" s="2" t="s">
+        <v>454</v>
+      </c>
+      <c r="G127" s="2" t="s">
+        <v>446</v>
+      </c>
+      <c r="L127" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="M127" s="2" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="128" spans="2:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="L128" s="2" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="129" spans="12:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="L129" s="2" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="130" spans="12:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="L130" s="2" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="131" spans="12:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="L131" s="2" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="132" spans="12:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="L132" s="2" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="133" spans="12:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="L133" s="2" t="s">
+        <v>364</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="V34:V49"/>
+    <mergeCell ref="AC2:AC17"/>
+    <mergeCell ref="AC18:AC33"/>
+    <mergeCell ref="AC34:AC48"/>
+    <mergeCell ref="O2:O11"/>
+    <mergeCell ref="O12:O22"/>
+    <mergeCell ref="H17:H32"/>
+    <mergeCell ref="V2:V17"/>
+    <mergeCell ref="V18:V33"/>
     <mergeCell ref="H33:H48"/>
     <mergeCell ref="A31:A45"/>
     <mergeCell ref="A16:A30"/>
     <mergeCell ref="A2:A15"/>
     <mergeCell ref="H2:H16"/>
-    <mergeCell ref="O2:O11"/>
-    <mergeCell ref="O12:O22"/>
-    <mergeCell ref="H17:H32"/>
-    <mergeCell ref="V2:V17"/>
-    <mergeCell ref="V18:V33"/>
-    <mergeCell ref="V34:V49"/>
-    <mergeCell ref="AC2:AC17"/>
-    <mergeCell ref="AC18:AC33"/>
-    <mergeCell ref="AC34:AC48"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>